<commit_message>
Agregar Ejemplo y cambios paciente
</commit_message>
<xml_diff>
--- a/output/CodeSystem-CSTipoIdentificador.xlsx
+++ b/output/CodeSystem-CSTipoIdentificador.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="80">
   <si>
     <t>Property</t>
   </si>
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>1.8.7</t>
+    <t>1.8.11</t>
   </si>
   <si>
     <t>Name</t>
@@ -123,91 +123,136 @@
     <t>Count</t>
   </si>
   <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>Level</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>Display</t>
+  </si>
+  <si>
+    <t>Definition</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>RUN</t>
+  </si>
+  <si>
+    <t>Rol Único Nacional</t>
+  </si>
+  <si>
+    <t>02</t>
+  </si>
+  <si>
+    <t>RUN Provisorio</t>
+  </si>
+  <si>
+    <t>RUN provisorio (Artículo 44)</t>
+  </si>
+  <si>
+    <t>03</t>
+  </si>
+  <si>
+    <t>RUN Madre</t>
+  </si>
+  <si>
+    <t>RUN Madre (para recién nacido)</t>
+  </si>
+  <si>
+    <t>04</t>
+  </si>
+  <si>
+    <t>Número Folio</t>
+  </si>
+  <si>
+    <t>Número Folio Comprobante de Parto chileno</t>
+  </si>
+  <si>
+    <t>05</t>
+  </si>
+  <si>
+    <t>PPN</t>
+  </si>
+  <si>
+    <t>Pasaporte</t>
+  </si>
+  <si>
+    <t>06</t>
+  </si>
+  <si>
+    <t>Documento de identificación del país de origen</t>
+  </si>
+  <si>
+    <t>07</t>
+  </si>
+  <si>
+    <t>Acta de nacimiento del país de origen</t>
+  </si>
+  <si>
+    <t>08</t>
+  </si>
+  <si>
+    <t>NIP</t>
+  </si>
+  <si>
+    <t>Número de Identificación Provisorio (NIP)</t>
+  </si>
+  <si>
+    <t>09</t>
+  </si>
+  <si>
+    <t>NIC</t>
+  </si>
+  <si>
+    <t>Número Identificatorio para cotizar (NIC)</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>IPA</t>
+  </si>
+  <si>
+    <t>Identificación Provisoria del Apoderado (IPA)</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>IPE</t>
+  </si>
+  <si>
+    <t>Identificación Provisoria del Escolar (IPE)</t>
+  </si>
+  <si>
     <t>12</t>
   </si>
   <si>
-    <t>Level</t>
-  </si>
-  <si>
-    <t>Code</t>
-  </si>
-  <si>
-    <t>Display</t>
-  </si>
-  <si>
-    <t>Definition</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>01</t>
-  </si>
-  <si>
-    <t>Rol Único Nacional o RUN</t>
-  </si>
-  <si>
-    <t>02</t>
-  </si>
-  <si>
-    <t>RUN provisorio (Artículo 44)</t>
-  </si>
-  <si>
-    <t>03</t>
-  </si>
-  <si>
-    <t>RUN madre (para recién nacido)</t>
-  </si>
-  <si>
-    <t>04</t>
-  </si>
-  <si>
-    <t>Número Folio Comprobante de Parto chileno</t>
-  </si>
-  <si>
-    <t>05</t>
-  </si>
-  <si>
-    <t>Pasaporte</t>
-  </si>
-  <si>
-    <t>06</t>
-  </si>
-  <si>
-    <t>Documento de identificación del país de origen</t>
-  </si>
-  <si>
-    <t>07</t>
-  </si>
-  <si>
-    <t>Acta de nacimiento del país de origen</t>
-  </si>
-  <si>
-    <t>08</t>
-  </si>
-  <si>
-    <t>Número de Identificación Provisorio (NIP)</t>
-  </si>
-  <si>
-    <t>09</t>
-  </si>
-  <si>
-    <t>Número Identificatorio para cotizar (NIC)</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>Identificación Provisoria del Apoderado (IPA)</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>Identificación Provisoria del Escolar (IPE)</t>
-  </si>
-  <si>
     <t>Número de Ficha Clínica Sistema Local</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>RNPI</t>
+  </si>
+  <si>
+    <t>Registro Nacional de Prestadores Individuales</t>
+  </si>
+  <si>
+    <t>OTRO</t>
+  </si>
+  <si>
+    <t>Otro tipo de identificador</t>
   </si>
 </sst>
 </file>
@@ -522,7 +567,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -552,139 +597,191 @@
       <c r="C2" t="s" s="2">
         <v>43</v>
       </c>
-      <c r="D2" s="2"/>
+      <c r="D2" t="s" s="2">
+        <v>44</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
         <v>41</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C3" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="D3" s="2"/>
+        <v>46</v>
+      </c>
+      <c r="D3" t="s" s="2">
+        <v>47</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
         <v>41</v>
       </c>
       <c r="B4" t="s" s="2">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C4" t="s" s="2">
-        <v>47</v>
-      </c>
-      <c r="D4" s="2"/>
+        <v>49</v>
+      </c>
+      <c r="D4" t="s" s="2">
+        <v>50</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="2">
         <v>41</v>
       </c>
       <c r="B5" t="s" s="2">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C5" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="D5" s="2"/>
+        <v>52</v>
+      </c>
+      <c r="D5" t="s" s="2">
+        <v>53</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="2">
         <v>41</v>
       </c>
       <c r="B6" t="s" s="2">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C6" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="D6" s="2"/>
+        <v>55</v>
+      </c>
+      <c r="D6" t="s" s="2">
+        <v>56</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="2">
         <v>41</v>
       </c>
       <c r="B7" t="s" s="2">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="C7" t="s" s="2">
-        <v>53</v>
-      </c>
-      <c r="D7" s="2"/>
+        <v>58</v>
+      </c>
+      <c r="D7" t="s" s="2">
+        <v>58</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="2">
         <v>41</v>
       </c>
       <c r="B8" t="s" s="2">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="C8" t="s" s="2">
-        <v>55</v>
-      </c>
-      <c r="D8" s="2"/>
+        <v>60</v>
+      </c>
+      <c r="D8" t="s" s="2">
+        <v>60</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="2">
         <v>41</v>
       </c>
       <c r="B9" t="s" s="2">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="C9" t="s" s="2">
-        <v>57</v>
-      </c>
-      <c r="D9" s="2"/>
+        <v>62</v>
+      </c>
+      <c r="D9" t="s" s="2">
+        <v>63</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="2">
         <v>41</v>
       </c>
       <c r="B10" t="s" s="2">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="C10" t="s" s="2">
-        <v>59</v>
-      </c>
-      <c r="D10" s="2"/>
+        <v>65</v>
+      </c>
+      <c r="D10" t="s" s="2">
+        <v>66</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="2">
         <v>41</v>
       </c>
       <c r="B11" t="s" s="2">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="C11" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="D11" s="2"/>
+        <v>68</v>
+      </c>
+      <c r="D11" t="s" s="2">
+        <v>69</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="2">
         <v>41</v>
       </c>
       <c r="B12" t="s" s="2">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="C12" t="s" s="2">
-        <v>63</v>
-      </c>
-      <c r="D12" s="2"/>
+        <v>71</v>
+      </c>
+      <c r="D12" t="s" s="2">
+        <v>72</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
         <v>41</v>
       </c>
       <c r="B13" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="C13" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="D13" t="s" s="2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="B14" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="C14" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="D14" t="s" s="2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="B15" t="s" s="2">
         <v>36</v>
       </c>
-      <c r="C13" t="s" s="2">
-        <v>64</v>
-      </c>
-      <c r="D13" s="2"/>
+      <c r="C15" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="D15" t="s" s="2">
+        <v>79</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>